<commit_message>
input parameters udated, small changes in batch steps
</commit_message>
<xml_diff>
--- a/samples_steps_template.xlsx
+++ b/samples_steps_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiia_hry/github/mpip/dex-stim-dna-methylation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7D5A3D-217E-8947-AC54-DD9F89807BDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4CD8F3-A527-3045-BC4D-553B3B3868C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1000" windowWidth="28800" windowHeight="16420" xr2:uid="{0E806724-001C-4148-A6ED-79CE17BF1AFD}"/>
+    <workbookView xWindow="0" yWindow="980" windowWidth="28800" windowHeight="16420" xr2:uid="{0E806724-001C-4148-A6ED-79CE17BF1AFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
   <si>
     <t>start RGSet (original)</t>
   </si>
@@ -108,12 +108,6 @@
     <t>PC3</t>
   </si>
   <si>
-    <t>Proportion variance</t>
-  </si>
-  <si>
-    <t>Cumulative variance</t>
-  </si>
-  <si>
     <t>PC4</t>
   </si>
   <si>
@@ -178,6 +172,69 @@
   </si>
   <si>
     <t>R06C01</t>
+  </si>
+  <si>
+    <t>PC6</t>
+  </si>
+  <si>
+    <t>PC7</t>
+  </si>
+  <si>
+    <t>PC8</t>
+  </si>
+  <si>
+    <t>PC9</t>
+  </si>
+  <si>
+    <t>PC10</t>
+  </si>
+  <si>
+    <t>PC11</t>
+  </si>
+  <si>
+    <t>PC12</t>
+  </si>
+  <si>
+    <t>PC13</t>
+  </si>
+  <si>
+    <t>PC14</t>
+  </si>
+  <si>
+    <t>PC15</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>0.74</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>0.60</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>0.52</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>Proportion variance (%)</t>
+  </si>
+  <si>
+    <t>Cumulative variance (%)</t>
   </si>
 </sst>
 </file>
@@ -187,7 +244,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,6 +347,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -345,7 +408,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -403,7 +466,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -420,6 +482,10 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -735,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7EF277-EC73-5843-8A8F-3EFAB31A65A1}">
-  <dimension ref="A2:G190"/>
+  <dimension ref="A2:U200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C138" sqref="B138:C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,14 +925,14 @@
       <c r="C23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="37"/>
+      <c r="E23" s="36"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E24" s="21"/>
     </row>
@@ -1010,8 +1076,8 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B51" s="19"/>
       <c r="C51" s="20"/>
-      <c r="D51" s="39" t="s">
-        <v>46</v>
+      <c r="D51" s="38" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1020,7 +1086,7 @@
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="34"/>
+      <c r="B53" s="33"/>
       <c r="C53" s="30"/>
       <c r="D53" s="6"/>
     </row>
@@ -1130,8 +1196,8 @@
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B74" s="10"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="39" t="s">
-        <v>46</v>
+      <c r="D74" s="38" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1156,13 +1222,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D79" s="26"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B80" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C80" s="27">
         <v>403</v>
@@ -1182,7 +1248,7 @@
       <c r="B82" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C82" s="40">
+      <c r="C82" s="39">
         <v>1052641</v>
       </c>
       <c r="D82" s="4"/>
@@ -1197,7 +1263,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C84" s="30"/>
     </row>
@@ -1223,7 +1289,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B88" s="32"/>
       <c r="C88" s="31"/>
@@ -1246,8 +1312,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="36" t="s">
-        <v>35</v>
+      <c r="A91" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="B91" s="28"/>
     </row>
@@ -1319,7 +1385,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -1374,7 +1440,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B113" s="13">
         <v>37869</v>
       </c>
@@ -1382,12 +1448,12 @@
         <v>751091</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A115" s="3"/>
       <c r="B115" s="7" t="s">
         <v>1</v>
@@ -1396,7 +1462,7 @@
         <v>751091</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B116" s="7" t="s">
         <v>2</v>
       </c>
@@ -1404,16 +1470,16 @@
         <v>403</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B117" s="32"/>
       <c r="C117" s="31"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B119" s="7" t="s">
         <v>15</v>
       </c>
@@ -1421,7 +1487,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B120" s="13">
         <v>447</v>
       </c>
@@ -1429,9 +1495,9 @@
         <v>750644</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>1</v>
@@ -1440,21 +1506,66 @@
         <v>750644</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B123" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C123" s="8">
         <v>447</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G123" s="41">
+        <v>30895</v>
+      </c>
+      <c r="H123" s="41">
+        <v>14001</v>
+      </c>
+      <c r="I123" s="41">
+        <v>18660</v>
+      </c>
+      <c r="J123" s="41">
+        <v>11355</v>
+      </c>
+      <c r="K123" s="41">
+        <v>11324</v>
+      </c>
+      <c r="L123" s="41">
+        <v>43831</v>
+      </c>
+      <c r="M123" t="s">
+        <v>59</v>
+      </c>
+      <c r="N123" t="s">
+        <v>60</v>
+      </c>
+      <c r="O123" t="s">
+        <v>61</v>
+      </c>
+      <c r="P123" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>63</v>
+      </c>
+      <c r="R123" t="s">
+        <v>64</v>
+      </c>
+      <c r="S123" t="s">
+        <v>65</v>
+      </c>
+      <c r="T123" t="s">
+        <v>66</v>
+      </c>
+      <c r="U123" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B125" s="41"/>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B125" s="40"/>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B126" s="7" t="s">
         <v>15</v>
       </c>
@@ -1462,17 +1573,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B127" s="35">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B127" s="34">
         <v>10287</v>
       </c>
       <c r="C127" s="14">
         <v>740357</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -1508,208 +1619,309 @@
       </c>
       <c r="B134" s="8"/>
       <c r="C134" s="7" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="D134" s="7" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B135" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C135" s="33"/>
-      <c r="D135" s="33"/>
+      <c r="C135" s="42">
+        <v>8.84</v>
+      </c>
+      <c r="D135" s="42">
+        <v>8.84</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B136" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C136" s="33"/>
-      <c r="D136" s="33"/>
+      <c r="C136" s="43">
+        <v>5.38</v>
+      </c>
+      <c r="D136" s="43">
+        <v>14.219999999999999</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B137" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C137" s="33"/>
-      <c r="D137" s="33"/>
+      <c r="C137" s="43">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="D137" s="43">
+        <v>16.729999999999997</v>
+      </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B138" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C138" s="33"/>
-      <c r="D138" s="33"/>
-      <c r="E138" s="38" t="s">
-        <v>47</v>
+        <v>27</v>
+      </c>
+      <c r="C138" s="43">
+        <v>2.31</v>
+      </c>
+      <c r="D138" s="43">
+        <v>19.039999999999996</v>
+      </c>
+      <c r="E138" s="37" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B139" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C139" s="8"/>
-      <c r="D139" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="C139" s="43">
+        <v>1.31</v>
+      </c>
+      <c r="D139" s="43">
+        <v>20.349999999999994</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B140" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C140" s="43">
+        <v>1.2</v>
+      </c>
+      <c r="D140" s="43">
+        <v>21.549999999999994</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
-        <v>37</v>
+      <c r="B141" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C141" s="44">
+        <v>0.98</v>
+      </c>
+      <c r="D141" s="44">
+        <v>22.529999999999994</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B142" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C142" s="8"/>
-      <c r="D142" s="31"/>
+        <v>51</v>
+      </c>
+      <c r="C142" s="44">
+        <v>0.93</v>
+      </c>
+      <c r="D142" s="44">
+        <v>23.459999999999994</v>
+      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B143" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C143" s="44">
+        <v>0.74</v>
+      </c>
+      <c r="D143" s="44">
+        <v>24.199999999999992</v>
+      </c>
+      <c r="E143" s="37"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B144" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C144" s="44">
+        <v>0.71</v>
+      </c>
+      <c r="D144" s="44">
+        <v>24.909999999999993</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B145" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C145" s="44">
+        <v>0.6</v>
+      </c>
+      <c r="D145" s="44">
+        <v>25.509999999999994</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B146" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C146" s="44">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D146" s="44">
+        <v>26.089999999999993</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B147" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C147" s="44">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D147" s="44">
+        <v>26.639999999999993</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B148" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C148" s="44">
+        <v>0.52</v>
+      </c>
+      <c r="D148" s="44">
+        <v>27.159999999999993</v>
+      </c>
+      <c r="E148" s="37"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B149" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C149" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="D149" s="44">
+        <v>27.659999999999993</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B152" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C152" s="8"/>
+      <c r="D152" s="31"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B153" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C143" s="8"/>
-      <c r="D143" s="31"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B144" s="32"/>
-      <c r="C144" s="31"/>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A145" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B145" s="32"/>
-      <c r="C145" s="31"/>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B146" s="7" t="s">
+      <c r="C153" s="8"/>
+      <c r="D153" s="31"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B154" s="32"/>
+      <c r="C154" s="31"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B155" s="32"/>
+      <c r="C155" s="31"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B156" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C146" s="7" t="s">
+      <c r="C156" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B147" s="8"/>
-      <c r="C147" s="8"/>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B148" s="8"/>
-      <c r="C148" s="8"/>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B149" s="8"/>
-      <c r="C149" s="13"/>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B150" s="8"/>
-      <c r="C150" s="8"/>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B151" s="8"/>
-      <c r="C151" s="13"/>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B152" s="8"/>
-      <c r="C152" s="8"/>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B153" s="8"/>
-      <c r="C153" s="8"/>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B156" s="8"/>
-      <c r="C156" s="8"/>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B159" s="7" t="s">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B159" s="8"/>
+      <c r="C159" s="13"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B160" s="8"/>
+      <c r="C160" s="8"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B161" s="8"/>
+      <c r="C161" s="13"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B162" s="8"/>
+      <c r="C162" s="8"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B163" s="8"/>
+      <c r="C163" s="8"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B164" s="8"/>
+      <c r="C164" s="8"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B165" s="8"/>
+      <c r="C165" s="8"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B166" s="8"/>
+      <c r="C166" s="8"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B167" s="8"/>
+      <c r="C167" s="8"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B168" s="8"/>
+      <c r="C168" s="8"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B169" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C169" s="7"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B172" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C172" s="9"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B173" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C173" s="9"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C159" s="7"/>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A161" s="1" t="s">
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B176" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B162" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C162" s="9"/>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B163" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C163" s="9"/>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A165" s="1" t="s">
+      <c r="C176" s="8"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B166" s="7" t="s">
+      <c r="B178" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C166" s="8"/>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A168" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B168" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B169" s="8"/>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B170" s="8"/>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B171" s="8"/>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B172" s="8"/>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B173" s="8"/>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B174" s="8"/>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B175" s="8"/>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B176" s="8"/>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B177" s="8"/>
-      <c r="C177" s="31"/>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B178" s="8"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B179" s="8"/>
@@ -1737,26 +1949,58 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B187" s="8"/>
-      <c r="C187" t="s">
-        <v>48</v>
-      </c>
+      <c r="C187" s="31"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B188" s="8"/>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A189" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B189" s="7" t="s">
+      <c r="B189" s="8"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B190" s="8"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B191" s="8"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B192" s="8"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B193" s="8"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B194" s="8"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B195" s="8"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B196" s="8"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B197" s="8"/>
+      <c r="C197" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B199" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C189" s="13"/>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B190" s="7" t="s">
+      <c r="C199" s="13"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B200" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C190" s="9"/>
+      <c r="C200" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
batch correction script updated
</commit_message>
<xml_diff>
--- a/samples_steps_template.xlsx
+++ b/samples_steps_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiia_hry/github/mpip/dex-stim-dna-methylation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4CD8F3-A527-3045-BC4D-553B3B3868C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF6BDE9-A84E-AB45-88A7-13E333E4B106}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="980" windowWidth="28800" windowHeight="16420" xr2:uid="{0E806724-001C-4148-A6ED-79CE17BF1AFD}"/>
   </bookViews>
@@ -804,7 +804,7 @@
   <dimension ref="A2:U200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C138" sqref="B138:C138"/>
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1804,14 +1804,18 @@
       <c r="B152" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C152" s="8"/>
+      <c r="C152" s="14">
+        <v>740357</v>
+      </c>
       <c r="D152" s="31"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B153" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C153" s="8"/>
+      <c r="C153" s="8">
+        <v>403</v>
+      </c>
       <c r="D153" s="31"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
some changes across the whole coed
</commit_message>
<xml_diff>
--- a/samples_steps_template.xlsx
+++ b/samples_steps_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiia_hry/bio/code/mpip/dex-stim-dna-methylation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87FE5FA-DE42-DC46-AE35-537A9731168B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C749F4-2136-B949-8EC9-55C2F257D9F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30420" yWindow="3320" windowWidth="38400" windowHeight="18000" xr2:uid="{0E806724-001C-4148-A6ED-79CE17BF1AFD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0E806724-001C-4148-A6ED-79CE17BF1AFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t>start RGSet (original)</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>MPIPSYKL_007893</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
@@ -758,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7EF277-EC73-5843-8A8F-3EFAB31A65A1}">
-  <dimension ref="A2:L121"/>
+  <dimension ref="A2:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1597,7 +1600,7 @@
         <v>38</v>
       </c>
       <c r="C117" s="7">
-        <v>1469</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -1605,23 +1608,28 @@
         <v>58</v>
       </c>
       <c r="C118" s="7">
-        <v>1439</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
+      <c r="A120" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B120" s="6" t="s">
+      <c r="B121" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C120" s="12"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B121" s="6" t="s">
+      <c r="C121" s="12"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B122" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C121" s="8"/>
+      <c r="C122" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>